<commit_message>
add columns to cell_all and change cellosaurus names
</commit_message>
<xml_diff>
--- a/cellosaurus_names.xlsx
+++ b/cellosaurus_names.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/psmirnov/IDrive-Sync/IDrive-Sync/macbook/Code/Github/pachyderm/Annotations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713D7439-2488-9949-B434-010212B2A1EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7AF3FF-23BD-F34D-B380-AB813ED95117}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10180" yWindow="5860" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="420" yWindow="1060" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cellosaurus_names" sheetId="1" r:id="rId1"/>
-    <sheet name="renaming2cellosaurus" sheetId="2" r:id="rId2"/>
+    <sheet name="deduplicate" sheetId="3" r:id="rId2"/>
+    <sheet name="renaming2cellosaurus" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">cellosaurus_names!$A$1:$F$1654</definedName>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13635" uniqueCount="5490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13703" uniqueCount="5496">
   <si>
     <t>cellosaurus_ac</t>
   </si>
@@ -16494,6 +16495,24 @@
   </si>
   <si>
     <t>PC-3_JPC-3</t>
+  </si>
+  <si>
+    <t>SJRH30</t>
+  </si>
+  <si>
+    <t>SJCRH30</t>
+  </si>
+  <si>
+    <t>TTTHYROID</t>
+  </si>
+  <si>
+    <t>NCI-H322T</t>
+  </si>
+  <si>
+    <t>MB157</t>
+  </si>
+  <si>
+    <t>MDAMB157</t>
   </si>
 </sst>
 </file>
@@ -17085,7 +17104,27 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -17413,8 +17452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1758"/>
   <sheetViews>
-    <sheetView topLeftCell="A1552" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D1569" sqref="D1:D1048576"/>
+    <sheetView topLeftCell="A1729" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B1737" sqref="B1737:C1737"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -46813,7 +46852,7 @@
   </sheetData>
   <autoFilter ref="A1:F1654" xr:uid="{F3E4B55C-1DD0-F14E-B3EB-ADFBEE217367}"/>
   <conditionalFormatting sqref="B1725 B1727:B1728">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -46821,10 +46860,303 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3909B46-42EB-6348-8AD4-13180313584F}">
+  <dimension ref="A1:B34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5355</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5350</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>5352</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5353</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5491</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5490</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5354</v>
+      </c>
+      <c r="B6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5357</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5358</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>495</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5359</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>501</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5360</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
+        <v>510</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5362</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
+        <v>590</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5473</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>5494</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>5495</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>5368</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
+        <v>1640</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5370</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>5371</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>5371</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>5493</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="13" t="s">
+        <v>2772</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5373</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
+        <v>2913</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5492</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="13" t="s">
+        <v>3121</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5374</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="13" t="s">
+        <v>3853</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5375</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>5376</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>4597</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>5377</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>4617</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="13" t="s">
+        <v>4700</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5378</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>5379</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>4784</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>5380</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>4787</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>5381</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>4790</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>5382</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>4797</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>5383</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>5067</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>5384</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>5074</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>5385</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>5077</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>5386</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>5080</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>5387</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>5083</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>3946</v>
+      </c>
+      <c r="B34" t="s">
+        <v>5398</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A3:A4">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C61D2288-C5AC-DF41-9472-A124A217A592}">
   <dimension ref="A1:E1717"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1550" workbookViewId="0">
+    <sheetView topLeftCell="A1887" workbookViewId="0">
       <selection activeCell="D1569" sqref="D1569"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Revert "fix cellosaurus names"
This reverts commit 7d8fa8ccdcc0d215b2e61d76c4c8971fc5c19922.
</commit_message>
<xml_diff>
--- a/cellosaurus_names.xlsx
+++ b/cellosaurus_names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/psmirnov/IDrive-Sync/IDrive-Sync/macbook/Code/Github/pachyderm/Annotations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7037F985-A07C-4343-B835-1662E9D7C83D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7AF3FF-23BD-F34D-B380-AB813ED95117}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11780" yWindow="16900" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="420" yWindow="1060" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cellosaurus_names" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13703" uniqueCount="5517">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13703" uniqueCount="5496">
   <si>
     <t>cellosaurus_ac</t>
   </si>
@@ -16513,69 +16513,6 @@
   </si>
   <si>
     <t>MDAMB157</t>
-  </si>
-  <si>
-    <t>U251_1628_2019</t>
-  </si>
-  <si>
-    <t>NCISNU16_1153_2019</t>
-  </si>
-  <si>
-    <t>NCISNU5_1154_2019</t>
-  </si>
-  <si>
-    <t>NCISNU1_1152_2019</t>
-  </si>
-  <si>
-    <t>Hs69ST_588_2019</t>
-  </si>
-  <si>
-    <t>U266_1620_2019</t>
-  </si>
-  <si>
-    <t>DOR13_305_2019</t>
-  </si>
-  <si>
-    <t>H322T_435_2019</t>
-  </si>
-  <si>
-    <t>H2373_421_2019</t>
-  </si>
-  <si>
-    <t>H2369_420_2019</t>
-  </si>
-  <si>
-    <t>H2461_422_2019</t>
-  </si>
-  <si>
-    <t>H2595_424_2019</t>
-  </si>
-  <si>
-    <t>H2722_425_2019</t>
-  </si>
-  <si>
-    <t>H2795_427_2019</t>
-  </si>
-  <si>
-    <t>H2803_428_2019</t>
-  </si>
-  <si>
-    <t>H2804_429_2019</t>
-  </si>
-  <si>
-    <t>H2810_430_2019</t>
-  </si>
-  <si>
-    <t>H3255_436_2019</t>
-  </si>
-  <si>
-    <t>HSTS_623_2019</t>
-  </si>
-  <si>
-    <t>KRIJ_792_2019</t>
-  </si>
-  <si>
-    <t>HCC812_511_2019</t>
   </si>
 </sst>
 </file>
@@ -17515,8 +17452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1758"/>
   <sheetViews>
-    <sheetView topLeftCell="A1154" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C1698" sqref="C1698"/>
+    <sheetView topLeftCell="A1729" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B1737" sqref="B1737:C1737"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -46924,10 +46861,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3909B46-42EB-6348-8AD4-13180313584F}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -47021,178 +46958,186 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>5494</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>5495</v>
+      <c r="A12" s="13" t="s">
+        <v>590</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5473</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>5494</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>5495</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>5368</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B14" s="13" t="s">
         <v>763</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="13" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
         <v>1640</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>5370</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>5371</v>
-      </c>
-      <c r="B15" t="s">
-        <v>2331</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>5371</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" t="s">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>5371</v>
+      </c>
+      <c r="B17" s="13" t="s">
         <v>5493</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="13" t="s">
-        <v>2772</v>
-      </c>
-      <c r="B17" t="s">
-        <v>5373</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
-        <v>2913</v>
+        <v>2772</v>
       </c>
       <c r="B18" t="s">
-        <v>5492</v>
+        <v>5373</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
-        <v>3121</v>
+        <v>2913</v>
       </c>
       <c r="B19" t="s">
-        <v>5374</v>
+        <v>5492</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
+        <v>3121</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5374</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="13" t="s">
         <v>3853</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>5375</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>5376</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>4597</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>5376</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>4597</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>5377</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B23" s="13" t="s">
         <v>4617</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="13" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="13" t="s">
         <v>4700</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>5378</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>5379</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>4784</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>5380</v>
+        <v>5379</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>4787</v>
+        <v>4784</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>5381</v>
+        <v>5380</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>4790</v>
+        <v>4787</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>5382</v>
+        <v>5381</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>4797</v>
+        <v>4790</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>5383</v>
+        <v>5382</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>5067</v>
+        <v>4797</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>5384</v>
+        <v>5383</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>5074</v>
+        <v>5067</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>5385</v>
+        <v>5384</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>5077</v>
+        <v>5074</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>5386</v>
+        <v>5385</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>5080</v>
+        <v>5077</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>5387</v>
+        <v>5386</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>5083</v>
+        <v>5080</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>5387</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>5083</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>3946</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>5398</v>
       </c>
     </row>
@@ -47211,17 +47156,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C61D2288-C5AC-DF41-9472-A124A217A592}">
   <dimension ref="A1:E1717"/>
   <sheetViews>
-    <sheetView topLeftCell="A1675" workbookViewId="0">
-      <selection activeCell="A1710" sqref="A1710:XFD1710"/>
+    <sheetView topLeftCell="A1887" workbookViewId="0">
+      <selection activeCell="D1569" sqref="D1569"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.5" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
@@ -47500,7 +47439,7 @@
         <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>5496</v>
+        <v>50</v>
       </c>
       <c r="D17" t="s">
         <v>51</v>
@@ -47976,7 +47915,7 @@
         <v>146</v>
       </c>
       <c r="C45" t="s">
-        <v>5497</v>
+        <v>147</v>
       </c>
       <c r="D45" t="s">
         <v>148</v>
@@ -48010,7 +47949,7 @@
         <v>5397</v>
       </c>
       <c r="C47" t="s">
-        <v>5498</v>
+        <v>152</v>
       </c>
       <c r="D47" t="s">
         <v>153</v>
@@ -48180,7 +48119,7 @@
         <v>181</v>
       </c>
       <c r="C57" t="s">
-        <v>5499</v>
+        <v>182</v>
       </c>
       <c r="D57" t="s">
         <v>183</v>
@@ -50390,7 +50329,7 @@
         <v>605</v>
       </c>
       <c r="C187" t="s">
-        <v>5501</v>
+        <v>606</v>
       </c>
       <c r="D187" t="s">
         <v>607</v>
@@ -51223,7 +51162,7 @@
         <v>761</v>
       </c>
       <c r="C236" t="s">
-        <v>5500</v>
+        <v>762</v>
       </c>
       <c r="D236" t="s">
         <v>763</v>
@@ -59553,7 +59492,7 @@
         <v>2329</v>
       </c>
       <c r="C726" t="s">
-        <v>5503</v>
+        <v>2330</v>
       </c>
       <c r="D726" t="s">
         <v>2331</v>
@@ -71674,7 +71613,7 @@
         <v>4595</v>
       </c>
       <c r="C1439" t="s">
-        <v>5502</v>
+        <v>4596</v>
       </c>
       <c r="D1439" t="s">
         <v>4597</v>
@@ -71776,7 +71715,7 @@
         <v>4615</v>
       </c>
       <c r="C1445" t="s">
-        <v>5513</v>
+        <v>4616</v>
       </c>
       <c r="D1445" t="s">
         <v>4617</v>
@@ -72592,7 +72531,7 @@
         <v>4782</v>
       </c>
       <c r="C1493" t="s">
-        <v>5505</v>
+        <v>4783</v>
       </c>
       <c r="D1493" t="s">
         <v>4784</v>
@@ -72609,7 +72548,7 @@
         <v>4785</v>
       </c>
       <c r="C1494" t="s">
-        <v>5504</v>
+        <v>4786</v>
       </c>
       <c r="D1494" t="s">
         <v>4787</v>
@@ -72626,7 +72565,7 @@
         <v>4788</v>
       </c>
       <c r="C1495" t="s">
-        <v>5506</v>
+        <v>4789</v>
       </c>
       <c r="D1495" t="s">
         <v>4790</v>
@@ -72660,7 +72599,7 @@
         <v>4795</v>
       </c>
       <c r="C1497" t="s">
-        <v>5507</v>
+        <v>4796</v>
       </c>
       <c r="D1497" t="s">
         <v>4797</v>
@@ -73357,7 +73296,7 @@
         <v>4936</v>
       </c>
       <c r="C1538" t="s">
-        <v>5514</v>
+        <v>4937</v>
       </c>
       <c r="D1538" t="s">
         <v>4937</v>
@@ -73952,7 +73891,7 @@
         <v>5065</v>
       </c>
       <c r="C1573" t="s">
-        <v>5508</v>
+        <v>5066</v>
       </c>
       <c r="D1573" t="s">
         <v>5067</v>
@@ -73986,7 +73925,7 @@
         <v>5072</v>
       </c>
       <c r="C1575" t="s">
-        <v>5509</v>
+        <v>5073</v>
       </c>
       <c r="D1575" t="s">
         <v>5074</v>
@@ -74003,7 +73942,7 @@
         <v>5075</v>
       </c>
       <c r="C1576" t="s">
-        <v>5510</v>
+        <v>5076</v>
       </c>
       <c r="D1576" t="s">
         <v>5077</v>
@@ -74020,7 +73959,7 @@
         <v>5078</v>
       </c>
       <c r="C1577" t="s">
-        <v>5511</v>
+        <v>5079</v>
       </c>
       <c r="D1577" t="s">
         <v>5080</v>
@@ -74037,7 +73976,7 @@
         <v>5081</v>
       </c>
       <c r="C1578" t="s">
-        <v>5512</v>
+        <v>5082</v>
       </c>
       <c r="D1578" t="s">
         <v>5083</v>
@@ -75634,9 +75573,6 @@
       <c r="A1681">
         <v>1680</v>
       </c>
-      <c r="C1681" t="s">
-        <v>5516</v>
-      </c>
       <c r="D1681" t="s">
         <v>5434</v>
       </c>
@@ -75680,9 +75616,6 @@
     <row r="1685" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1685">
         <v>1684</v>
-      </c>
-      <c r="C1685" t="s">
-        <v>5515</v>
       </c>
       <c r="D1685" t="s">
         <v>5439</v>

</xml_diff>

<commit_message>
Revert "Revert "fix cellosaurus names""
This reverts commit dd4388567429f60615a60780e0d5f7f6a287db80.
</commit_message>
<xml_diff>
--- a/cellosaurus_names.xlsx
+++ b/cellosaurus_names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/psmirnov/IDrive-Sync/IDrive-Sync/macbook/Code/Github/pachyderm/Annotations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7AF3FF-23BD-F34D-B380-AB813ED95117}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7037F985-A07C-4343-B835-1662E9D7C83D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="1060" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11780" yWindow="16900" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cellosaurus_names" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13703" uniqueCount="5496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13703" uniqueCount="5517">
   <si>
     <t>cellosaurus_ac</t>
   </si>
@@ -16513,6 +16513,69 @@
   </si>
   <si>
     <t>MDAMB157</t>
+  </si>
+  <si>
+    <t>U251_1628_2019</t>
+  </si>
+  <si>
+    <t>NCISNU16_1153_2019</t>
+  </si>
+  <si>
+    <t>NCISNU5_1154_2019</t>
+  </si>
+  <si>
+    <t>NCISNU1_1152_2019</t>
+  </si>
+  <si>
+    <t>Hs69ST_588_2019</t>
+  </si>
+  <si>
+    <t>U266_1620_2019</t>
+  </si>
+  <si>
+    <t>DOR13_305_2019</t>
+  </si>
+  <si>
+    <t>H322T_435_2019</t>
+  </si>
+  <si>
+    <t>H2373_421_2019</t>
+  </si>
+  <si>
+    <t>H2369_420_2019</t>
+  </si>
+  <si>
+    <t>H2461_422_2019</t>
+  </si>
+  <si>
+    <t>H2595_424_2019</t>
+  </si>
+  <si>
+    <t>H2722_425_2019</t>
+  </si>
+  <si>
+    <t>H2795_427_2019</t>
+  </si>
+  <si>
+    <t>H2803_428_2019</t>
+  </si>
+  <si>
+    <t>H2804_429_2019</t>
+  </si>
+  <si>
+    <t>H2810_430_2019</t>
+  </si>
+  <si>
+    <t>H3255_436_2019</t>
+  </si>
+  <si>
+    <t>HSTS_623_2019</t>
+  </si>
+  <si>
+    <t>KRIJ_792_2019</t>
+  </si>
+  <si>
+    <t>HCC812_511_2019</t>
   </si>
 </sst>
 </file>
@@ -17452,8 +17515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1758"/>
   <sheetViews>
-    <sheetView topLeftCell="A1729" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B1737" sqref="B1737:C1737"/>
+    <sheetView topLeftCell="A1154" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C1698" sqref="C1698"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -46861,10 +46924,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3909B46-42EB-6348-8AD4-13180313584F}">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -46958,186 +47021,178 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="13" t="s">
-        <v>590</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5473</v>
+      <c r="A12" t="s">
+        <v>5494</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>5495</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>5494</v>
+        <v>5368</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>5495</v>
+        <v>763</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>5368</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>763</v>
+      <c r="A14" s="13" t="s">
+        <v>1640</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5370</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="13" t="s">
-        <v>1640</v>
+      <c r="A15" t="s">
+        <v>5371</v>
       </c>
       <c r="B15" t="s">
-        <v>5370</v>
+        <v>2331</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>5371</v>
       </c>
-      <c r="B16" t="s">
-        <v>2331</v>
+      <c r="B16" s="13" t="s">
+        <v>5493</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>5371</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>5493</v>
+      <c r="A17" s="13" t="s">
+        <v>2772</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5373</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
-        <v>2772</v>
+        <v>2913</v>
       </c>
       <c r="B18" t="s">
-        <v>5373</v>
+        <v>5492</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
-        <v>2913</v>
+        <v>3121</v>
       </c>
       <c r="B19" t="s">
-        <v>5492</v>
+        <v>5374</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
-        <v>3121</v>
+        <v>3853</v>
       </c>
       <c r="B20" t="s">
-        <v>5374</v>
+        <v>5375</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="13" t="s">
-        <v>3853</v>
-      </c>
-      <c r="B21" t="s">
-        <v>5375</v>
+      <c r="A21" t="s">
+        <v>5376</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>4597</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>5376</v>
+        <v>5377</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>4597</v>
+        <v>4617</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>5377</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>4617</v>
+      <c r="A23" s="13" t="s">
+        <v>4700</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5378</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="13" t="s">
-        <v>4700</v>
-      </c>
-      <c r="B24" t="s">
-        <v>5378</v>
+      <c r="A24" t="s">
+        <v>5379</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>4784</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>5379</v>
+        <v>5380</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>4784</v>
+        <v>4787</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>5380</v>
+        <v>5381</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>4787</v>
+        <v>4790</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>5381</v>
+        <v>5382</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>4790</v>
+        <v>4797</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>5382</v>
+        <v>5383</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>4797</v>
+        <v>5067</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>5383</v>
+        <v>5384</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>5067</v>
+        <v>5074</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>5384</v>
+        <v>5385</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>5074</v>
+        <v>5077</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>5385</v>
+        <v>5386</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>5077</v>
+        <v>5080</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>5386</v>
+        <v>5387</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>5080</v>
+        <v>5083</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>5387</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>5083</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
         <v>3946</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B33" t="s">
         <v>5398</v>
       </c>
     </row>
@@ -47156,11 +47211,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C61D2288-C5AC-DF41-9472-A124A217A592}">
   <dimension ref="A1:E1717"/>
   <sheetViews>
-    <sheetView topLeftCell="A1887" workbookViewId="0">
-      <selection activeCell="D1569" sqref="D1569"/>
+    <sheetView topLeftCell="A1675" workbookViewId="0">
+      <selection activeCell="A1710" sqref="A1710:XFD1710"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
@@ -47439,7 +47500,7 @@
         <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>5496</v>
       </c>
       <c r="D17" t="s">
         <v>51</v>
@@ -47915,7 +47976,7 @@
         <v>146</v>
       </c>
       <c r="C45" t="s">
-        <v>147</v>
+        <v>5497</v>
       </c>
       <c r="D45" t="s">
         <v>148</v>
@@ -47949,7 +48010,7 @@
         <v>5397</v>
       </c>
       <c r="C47" t="s">
-        <v>152</v>
+        <v>5498</v>
       </c>
       <c r="D47" t="s">
         <v>153</v>
@@ -48119,7 +48180,7 @@
         <v>181</v>
       </c>
       <c r="C57" t="s">
-        <v>182</v>
+        <v>5499</v>
       </c>
       <c r="D57" t="s">
         <v>183</v>
@@ -50329,7 +50390,7 @@
         <v>605</v>
       </c>
       <c r="C187" t="s">
-        <v>606</v>
+        <v>5501</v>
       </c>
       <c r="D187" t="s">
         <v>607</v>
@@ -51162,7 +51223,7 @@
         <v>761</v>
       </c>
       <c r="C236" t="s">
-        <v>762</v>
+        <v>5500</v>
       </c>
       <c r="D236" t="s">
         <v>763</v>
@@ -59492,7 +59553,7 @@
         <v>2329</v>
       </c>
       <c r="C726" t="s">
-        <v>2330</v>
+        <v>5503</v>
       </c>
       <c r="D726" t="s">
         <v>2331</v>
@@ -71613,7 +71674,7 @@
         <v>4595</v>
       </c>
       <c r="C1439" t="s">
-        <v>4596</v>
+        <v>5502</v>
       </c>
       <c r="D1439" t="s">
         <v>4597</v>
@@ -71715,7 +71776,7 @@
         <v>4615</v>
       </c>
       <c r="C1445" t="s">
-        <v>4616</v>
+        <v>5513</v>
       </c>
       <c r="D1445" t="s">
         <v>4617</v>
@@ -72531,7 +72592,7 @@
         <v>4782</v>
       </c>
       <c r="C1493" t="s">
-        <v>4783</v>
+        <v>5505</v>
       </c>
       <c r="D1493" t="s">
         <v>4784</v>
@@ -72548,7 +72609,7 @@
         <v>4785</v>
       </c>
       <c r="C1494" t="s">
-        <v>4786</v>
+        <v>5504</v>
       </c>
       <c r="D1494" t="s">
         <v>4787</v>
@@ -72565,7 +72626,7 @@
         <v>4788</v>
       </c>
       <c r="C1495" t="s">
-        <v>4789</v>
+        <v>5506</v>
       </c>
       <c r="D1495" t="s">
         <v>4790</v>
@@ -72599,7 +72660,7 @@
         <v>4795</v>
       </c>
       <c r="C1497" t="s">
-        <v>4796</v>
+        <v>5507</v>
       </c>
       <c r="D1497" t="s">
         <v>4797</v>
@@ -73296,7 +73357,7 @@
         <v>4936</v>
       </c>
       <c r="C1538" t="s">
-        <v>4937</v>
+        <v>5514</v>
       </c>
       <c r="D1538" t="s">
         <v>4937</v>
@@ -73891,7 +73952,7 @@
         <v>5065</v>
       </c>
       <c r="C1573" t="s">
-        <v>5066</v>
+        <v>5508</v>
       </c>
       <c r="D1573" t="s">
         <v>5067</v>
@@ -73925,7 +73986,7 @@
         <v>5072</v>
       </c>
       <c r="C1575" t="s">
-        <v>5073</v>
+        <v>5509</v>
       </c>
       <c r="D1575" t="s">
         <v>5074</v>
@@ -73942,7 +74003,7 @@
         <v>5075</v>
       </c>
       <c r="C1576" t="s">
-        <v>5076</v>
+        <v>5510</v>
       </c>
       <c r="D1576" t="s">
         <v>5077</v>
@@ -73959,7 +74020,7 @@
         <v>5078</v>
       </c>
       <c r="C1577" t="s">
-        <v>5079</v>
+        <v>5511</v>
       </c>
       <c r="D1577" t="s">
         <v>5080</v>
@@ -73976,7 +74037,7 @@
         <v>5081</v>
       </c>
       <c r="C1578" t="s">
-        <v>5082</v>
+        <v>5512</v>
       </c>
       <c r="D1578" t="s">
         <v>5083</v>
@@ -75573,6 +75634,9 @@
       <c r="A1681">
         <v>1680</v>
       </c>
+      <c r="C1681" t="s">
+        <v>5516</v>
+      </c>
       <c r="D1681" t="s">
         <v>5434</v>
       </c>
@@ -75616,6 +75680,9 @@
     <row r="1685" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1685">
         <v>1684</v>
+      </c>
+      <c r="C1685" t="s">
+        <v>5515</v>
       </c>
       <c r="D1685" t="s">
         <v>5439</v>

</xml_diff>

<commit_message>
fix some small misssing values in the two files
</commit_message>
<xml_diff>
--- a/cellosaurus_names.xlsx
+++ b/cellosaurus_names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/psmirnov/IDrive-Sync/IDrive-Sync/macbook/Code/Github/pachyderm/Annotations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7037F985-A07C-4343-B835-1662E9D7C83D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5785AF79-DA36-9942-B558-F0290233644E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11780" yWindow="16900" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11780" yWindow="16900" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cellosaurus_names" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13703" uniqueCount="5517">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13704" uniqueCount="5518">
   <si>
     <t>cellosaurus_ac</t>
   </si>
@@ -16576,6 +16576,9 @@
   </si>
   <si>
     <t>HCC812_511_2019</t>
+  </si>
+  <si>
+    <t>T47D_KBluc_1560_2019</t>
   </si>
 </sst>
 </file>
@@ -46926,7 +46929,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3909B46-42EB-6348-8AD4-13180313584F}">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
@@ -47211,8 +47214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C61D2288-C5AC-DF41-9472-A124A217A592}">
   <dimension ref="A1:E1717"/>
   <sheetViews>
-    <sheetView topLeftCell="A1675" workbookViewId="0">
-      <selection activeCell="A1710" sqref="A1710:XFD1710"/>
+    <sheetView tabSelected="1" topLeftCell="A1679" workbookViewId="0">
+      <selection activeCell="C1710" sqref="C1710"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -75959,6 +75962,9 @@
       <c r="A1710">
         <v>1709</v>
       </c>
+      <c r="C1710" t="s">
+        <v>5517</v>
+      </c>
       <c r="D1710" t="s">
         <v>5473</v>
       </c>

</xml_diff>